<commit_message>
add data-block and map block
</commit_message>
<xml_diff>
--- a/dats/kirov.xlsx
+++ b/dats/kirov.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">address</t>
   </si>
@@ -40,16 +40,7 @@
     <t xml:space="preserve">Киров Пугачева 5</t>
   </si>
   <si>
-    <t xml:space="preserve">Киров Пугачева 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Киров Пугачева 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Киров Пугачева 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Киров Пугачева 9</t>
+    <t xml:space="preserve">Киров Пугачева 11111</t>
   </si>
 </sst>
 </file>
@@ -146,10 +137,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -192,21 +183,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>